<commit_message>
Refactored directory stuff and made progress on loading a report.
</commit_message>
<xml_diff>
--- a/Grading/example grading output.xlsx
+++ b/Grading/example grading output.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t xml:space="preserve">Last Name</t>
   </si>
@@ -41,6 +41,12 @@
     <t xml:space="preserve">Part 2</t>
   </si>
   <si>
+    <t xml:space="preserve">Test 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bedwell</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
     <t xml:space="preserve">Security Issue</t>
   </si>
   <si>
+    <t xml:space="preserve">Fail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Johnson</t>
   </si>
   <si>
@@ -62,6 +71,9 @@
     <t xml:space="preserve">danigirl</t>
   </si>
   <si>
+    <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">Average</t>
   </si>
   <si>
@@ -80,10 +92,16 @@
     <t xml:space="preserve">Standard Deviation</t>
   </si>
   <si>
-    <t xml:space="preserve">Pass test 1 %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pass test 2 %</t>
+    <t xml:space="preserve">Part 1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 2 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 1 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test 2 %</t>
   </si>
 </sst>
 </file>
@@ -98,6 +116,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,8 +176,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,72 +202,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -266,206 +307,135 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>2.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>4</v>
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="0" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="A19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>50</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>0</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>5</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>5</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>2</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>50</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>50</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>